<commit_message>
Mac local changes - mostly updating figures
</commit_message>
<xml_diff>
--- a/averaged_runsNorESM copy.xlsx
+++ b/averaged_runsNorESM copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JohnMatthew/Downloads/Thorne_15_codefigurestats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8E4A64-1A34-7B4E-A862-EF7C51F73770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B28E8F-3557-9842-8B6B-8E87E85B83CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54180" yWindow="-2460" windowWidth="27240" windowHeight="16440" xr2:uid="{AB87CD62-F563-BD4E-A04A-E4844F3BBEB6}"/>
+    <workbookView xWindow="18620" yWindow="500" windowWidth="35840" windowHeight="21200" xr2:uid="{AB87CD62-F563-BD4E-A04A-E4844F3BBEB6}"/>
   </bookViews>
   <sheets>
     <sheet name="averaged_runsVolc" sheetId="1" r:id="rId1"/>
@@ -371,7 +371,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -875,10 +875,10 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1257,10 +1257,10 @@
   <dimension ref="A1:AU61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AO25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AJ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ31" sqref="AQ31"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1418,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <f>AT2</f>
+        <f t="shared" ref="D2:D33" si="0">AT2</f>
         <v>0</v>
       </c>
       <c r="E2" t="s">
@@ -1545,11 +1545,11 @@
         <v>0.13229042898235799</v>
       </c>
       <c r="AT2">
-        <f>(AR2&lt;$AT$1)*1</f>
+        <f t="shared" ref="AT2:AT33" si="1">(AR2&lt;$AT$1)*1</f>
         <v>0</v>
       </c>
       <c r="AU2">
-        <f>(AS2&lt;$AT$1)*1</f>
+        <f t="shared" ref="AU2:AU33" si="2">(AS2&lt;$AT$1)*1</f>
         <v>0</v>
       </c>
     </row>
@@ -1565,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f>AT3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E3" t="s">
@@ -1692,11 +1692,11 @@
         <v>0.12954812640233601</v>
       </c>
       <c r="AT3">
-        <f>(AR3&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU3">
-        <f>(AS3&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1712,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f>AT4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" t="s">
@@ -1839,11 +1839,11 @@
         <v>0.16031932416031999</v>
       </c>
       <c r="AT4">
-        <f>(AR4&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU4">
-        <f>(AS4&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <f>AT5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E5" t="s">
@@ -1986,11 +1986,11 @@
         <v>0.13188461882088101</v>
       </c>
       <c r="AT5">
-        <f>(AR5&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU5">
-        <f>(AS5&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2006,7 +2006,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <f>AT6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" t="s">
@@ -2133,11 +2133,11 @@
         <v>0.130823569222903</v>
       </c>
       <c r="AT6">
-        <f>(AR6&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU6">
-        <f>(AS6&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2153,7 +2153,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f>AT7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7" t="s">
@@ -2280,11 +2280,11 @@
         <v>9.6979883491678506E-2</v>
       </c>
       <c r="AT7">
-        <f>(AR7&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU7">
-        <f>(AS7&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2300,7 +2300,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f>AT8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8" t="s">
@@ -2427,11 +2427,11 @@
         <v>0.10681616995559801</v>
       </c>
       <c r="AT8">
-        <f>(AR8&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU8">
-        <f>(AS8&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2447,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f>AT9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E9" t="s">
@@ -2574,11 +2574,11 @@
         <v>0.29265891995059401</v>
       </c>
       <c r="AT9">
-        <f>(AR9&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU9">
-        <f>(AS9&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2594,7 +2594,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <f>AT10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E10" t="s">
@@ -2721,11 +2721,11 @@
         <v>0.14242502865203099</v>
       </c>
       <c r="AT10">
-        <f>(AR10&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU10">
-        <f>(AS10&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2741,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f>AT11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" t="s">
@@ -2868,11 +2868,11 @@
         <v>0.112653702661011</v>
       </c>
       <c r="AT11">
-        <f>(AR11&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU11">
-        <f>(AS11&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2888,7 +2888,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f>AT12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E12" t="s">
@@ -3015,11 +3015,11 @@
         <v>0.14309045191276801</v>
       </c>
       <c r="AT12">
-        <f>(AR12&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU12">
-        <f>(AS12&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3035,7 +3035,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <f>AT13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E13" t="s">
@@ -3162,11 +3162,11 @@
         <v>0.12099814073744899</v>
       </c>
       <c r="AT13">
-        <f>(AR13&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU13">
-        <f>(AS13&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3182,7 +3182,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <f>AT14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E14" t="s">
@@ -3309,11 +3309,11 @@
         <v>0.12180876298783</v>
       </c>
       <c r="AT14">
-        <f>(AR14&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU14">
-        <f>(AS14&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3329,7 +3329,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="3">
-        <f>AT15</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -3456,11 +3456,11 @@
         <v>0.11772251002480701</v>
       </c>
       <c r="AT15" s="3">
-        <f>(AR15&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AU15" s="3">
-        <f>(AS15&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3476,7 +3476,7 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <f>AT16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E16" t="s">
@@ -3603,11 +3603,11 @@
         <v>0.15450498391078599</v>
       </c>
       <c r="AT16">
-        <f>(AR16&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU16">
-        <f>(AS16&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3623,7 +3623,7 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <f>AT17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E17" t="s">
@@ -3750,11 +3750,11 @@
         <v>0.14361291864269901</v>
       </c>
       <c r="AT17">
-        <f>(AR17&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU17">
-        <f>(AS17&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3770,7 +3770,7 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <f>AT18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E18" t="s">
@@ -3897,11 +3897,11 @@
         <v>0.14361291864269901</v>
       </c>
       <c r="AT18">
-        <f>(AR18&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU18">
-        <f>(AS18&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3917,7 +3917,7 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <f>AT19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E19" t="s">
@@ -4044,11 +4044,11 @@
         <v>0.14361291864269901</v>
       </c>
       <c r="AT19">
-        <f>(AR19&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU19">
-        <f>(AS19&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4064,7 +4064,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <f>AT20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E20" t="s">
@@ -4191,11 +4191,11 @@
         <v>0.133557129874248</v>
       </c>
       <c r="AT20">
-        <f>(AR20&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU20">
-        <f>(AS20&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4211,7 +4211,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <f>AT21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E21" t="s">
@@ -4338,11 +4338,11 @@
         <v>0.159324485331275</v>
       </c>
       <c r="AT21">
-        <f>(AR21&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU21">
-        <f>(AS21&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4358,7 +4358,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="2">
-        <f>AT22</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E22" t="s">
@@ -4485,11 +4485,11 @@
         <v>0.11021092686558601</v>
       </c>
       <c r="AT22">
-        <f>(AR22&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AU22">
-        <f>(AS22&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4505,7 +4505,7 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <f>AT23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E23" t="s">
@@ -4632,11 +4632,11 @@
         <v>0.14637634728434101</v>
       </c>
       <c r="AT23">
-        <f>(AR23&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU23">
-        <f>(AS23&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4652,7 +4652,7 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <f>AT24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E24" t="s">
@@ -4779,11 +4779,11 @@
         <v>0.14716113303964501</v>
       </c>
       <c r="AT24">
-        <f>(AR24&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU24">
-        <f>(AS24&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4799,7 +4799,7 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <f>AT25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E25" t="s">
@@ -4926,11 +4926,11 @@
         <v>0.12744230424752401</v>
       </c>
       <c r="AT25">
-        <f>(AR25&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU25">
-        <f>(AS25&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4946,7 +4946,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="3">
-        <f>AT26</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -5073,11 +5073,11 @@
         <v>0.113944467847533</v>
       </c>
       <c r="AT26" s="3">
-        <f>(AR26&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AU26" s="3">
-        <f>(AS26&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5093,7 +5093,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="3">
-        <f>AT27</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -5220,11 +5220,11 @@
         <v>0.122318044546222</v>
       </c>
       <c r="AT27" s="3">
-        <f>(AR27&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AU27" s="3">
-        <f>(AS27&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5240,7 +5240,7 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <f>AT28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E28" t="s">
@@ -5367,11 +5367,11 @@
         <v>0.130559988576393</v>
       </c>
       <c r="AT28">
-        <f>(AR28&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU28">
-        <f>(AS28&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5387,7 +5387,7 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <f>AT29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E29" t="s">
@@ -5514,11 +5514,11 @@
         <v>0.121506624219184</v>
       </c>
       <c r="AT29">
-        <f>(AR29&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU29">
-        <f>(AS29&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5534,7 +5534,7 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <f>AT30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E30" t="s">
@@ -5661,11 +5661,11 @@
         <v>0.135511955330094</v>
       </c>
       <c r="AT30">
-        <f>(AR30&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU30">
-        <f>(AS30&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5681,7 +5681,7 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <f>AT31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E31" t="s">
@@ -5808,11 +5808,11 @@
         <v>0.131849630255823</v>
       </c>
       <c r="AT31">
-        <f>(AR31&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU31">
-        <f>(AS31&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5828,7 +5828,7 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <f>AT32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E32" t="s">
@@ -5955,11 +5955,11 @@
         <v>0.15855305208075801</v>
       </c>
       <c r="AT32">
-        <f>(AR32&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU32">
-        <f>(AS32&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5975,7 +5975,7 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <f>AT33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E33" t="s">
@@ -6102,11 +6102,11 @@
         <v>0.15629280991370301</v>
       </c>
       <c r="AT33">
-        <f>(AR33&lt;$AT$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU33">
-        <f>(AS33&lt;$AT$1)*1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6122,7 +6122,7 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <f>AT34</f>
+        <f t="shared" ref="D34:D56" si="3">AT34</f>
         <v>0</v>
       </c>
       <c r="E34" t="s">
@@ -6249,11 +6249,11 @@
         <v>0.15129884924727699</v>
       </c>
       <c r="AT34">
-        <f>(AR34&lt;$AT$1)*1</f>
+        <f t="shared" ref="AT34:AT56" si="4">(AR34&lt;$AT$1)*1</f>
         <v>0</v>
       </c>
       <c r="AU34">
-        <f>(AS34&lt;$AT$1)*1</f>
+        <f t="shared" ref="AU34:AU56" si="5">(AS34&lt;$AT$1)*1</f>
         <v>0</v>
       </c>
     </row>
@@ -6269,7 +6269,7 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <f>AT35</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E35" t="s">
@@ -6396,11 +6396,11 @@
         <v>0.201851518694624</v>
       </c>
       <c r="AT35">
-        <f>(AR35&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU35">
-        <f>(AS35&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6416,7 +6416,7 @@
         <v>0</v>
       </c>
       <c r="D36">
-        <f>AT36</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E36" t="s">
@@ -6543,11 +6543,11 @@
         <v>0.25438510713214202</v>
       </c>
       <c r="AT36">
-        <f>(AR36&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU36">
-        <f>(AS36&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6563,7 +6563,7 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <f>AT37</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E37" t="s">
@@ -6690,11 +6690,11 @@
         <v>0.16695424470621401</v>
       </c>
       <c r="AT37">
-        <f>(AR37&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU37">
-        <f>(AS37&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6710,7 +6710,7 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <f>AT38</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E38" t="s">
@@ -6837,11 +6837,11 @@
         <v>0.12062142503751901</v>
       </c>
       <c r="AT38">
-        <f>(AR38&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU38">
-        <f>(AS38&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6857,7 +6857,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="7">
-        <f>AT39</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E39" s="7" t="s">
@@ -6984,11 +6984,11 @@
         <v>7.3944819360348898E-2</v>
       </c>
       <c r="AT39" s="7">
-        <f>(AR39&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU39" s="7">
-        <f>(AS39&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7004,7 +7004,7 @@
         <v>0</v>
       </c>
       <c r="D40" s="3">
-        <f>AT40</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -7131,11 +7131,11 @@
         <v>9.2308757493555604E-2</v>
       </c>
       <c r="AT40" s="3">
-        <f>(AR40&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AU40" s="3">
-        <f>(AS40&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7151,7 +7151,7 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <f>AT41</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E41" t="s">
@@ -7278,11 +7278,11 @@
         <v>0.12932471909842999</v>
       </c>
       <c r="AT41">
-        <f>(AR41&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU41">
-        <f>(AS41&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7298,7 +7298,7 @@
         <v>0</v>
       </c>
       <c r="D42" s="3">
-        <f>AT42</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -7425,11 +7425,11 @@
         <v>7.2032659005548505E-2</v>
       </c>
       <c r="AT42" s="3">
-        <f>(AR42&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU42" s="3">
-        <f>(AS42&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -7445,7 +7445,7 @@
         <v>0</v>
       </c>
       <c r="D43">
-        <f>AT43</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E43" t="s">
@@ -7572,11 +7572,11 @@
         <v>0.14720799934915299</v>
       </c>
       <c r="AT43">
-        <f>(AR43&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU43">
-        <f>(AS43&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7592,7 +7592,7 @@
         <v>0</v>
       </c>
       <c r="D44">
-        <f>AT44</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E44" t="s">
@@ -7719,11 +7719,11 @@
         <v>0.182711394382956</v>
       </c>
       <c r="AT44">
-        <f>(AR44&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU44">
-        <f>(AS44&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7739,7 +7739,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="3">
-        <f>AT45</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -7866,11 +7866,11 @@
         <v>8.2646223633168106E-2</v>
       </c>
       <c r="AT45" s="3">
-        <f>(AR45&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AU45" s="3">
-        <f>(AS45&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7886,7 +7886,7 @@
         <v>0</v>
       </c>
       <c r="D46">
-        <f>AT46</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E46" t="s">
@@ -8013,11 +8013,11 @@
         <v>0.21450398661119999</v>
       </c>
       <c r="AT46">
-        <f>(AR46&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU46">
-        <f>(AS46&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8033,7 +8033,7 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <f>AT47</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E47" t="s">
@@ -8160,11 +8160,11 @@
         <v>0.27813358112497899</v>
       </c>
       <c r="AT47">
-        <f>(AR47&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU47">
-        <f>(AS47&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8180,7 +8180,7 @@
         <v>0</v>
       </c>
       <c r="D48">
-        <f>AT48</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E48" t="s">
@@ -8307,11 +8307,11 @@
         <v>0.20960436346814901</v>
       </c>
       <c r="AT48">
-        <f>(AR48&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU48">
-        <f>(AS48&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8327,7 +8327,7 @@
         <v>0</v>
       </c>
       <c r="D49" s="3">
-        <f>AT49</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -8454,11 +8454,11 @@
         <v>5.7663962789927803E-2</v>
       </c>
       <c r="AT49" s="3">
-        <f>(AR49&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU49" s="3">
-        <f>(AS49&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -8474,7 +8474,7 @@
         <v>0</v>
       </c>
       <c r="D50">
-        <f>AT50</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E50" t="s">
@@ -8601,11 +8601,11 @@
         <v>0.27183656755810298</v>
       </c>
       <c r="AT50">
-        <f>(AR50&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU50">
-        <f>(AS50&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8621,7 +8621,7 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <f>AT51</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E51" t="s">
@@ -8748,11 +8748,11 @@
         <v>0.32809491359637599</v>
       </c>
       <c r="AT51">
-        <f>(AR51&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU51">
-        <f>(AS51&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8768,7 +8768,7 @@
         <v>0</v>
       </c>
       <c r="D52">
-        <f>AT52</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E52" t="s">
@@ -8895,11 +8895,11 @@
         <v>0.25746174980125702</v>
       </c>
       <c r="AT52">
-        <f>(AR52&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU52">
-        <f>(AS52&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8915,7 +8915,7 @@
         <v>0</v>
       </c>
       <c r="D53">
-        <f>AT53</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E53" t="s">
@@ -9042,11 +9042,11 @@
         <v>0.26996358653378</v>
       </c>
       <c r="AT53">
-        <f>(AR53&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU53">
-        <f>(AS53&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9062,7 +9062,7 @@
         <v>0</v>
       </c>
       <c r="D54">
-        <f>AT54</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E54" t="s">
@@ -9189,11 +9189,11 @@
         <v>0.14469252911983499</v>
       </c>
       <c r="AT54">
-        <f>(AR54&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU54">
-        <f>(AS54&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9209,7 +9209,7 @@
         <v>1</v>
       </c>
       <c r="D55" s="3">
-        <f>AT55</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E55" s="3" t="s">
@@ -9336,11 +9336,11 @@
         <v>0.118524919970176</v>
       </c>
       <c r="AT55" s="3">
-        <f>(AR55&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AU55" s="3">
-        <f>(AS55&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9356,7 +9356,7 @@
         <v>0</v>
       </c>
       <c r="D56">
-        <f>AT56</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E56" t="s">
@@ -9483,11 +9483,11 @@
         <v>0.121882743634084</v>
       </c>
       <c r="AT56">
-        <f>(AR56&lt;$AT$1)*1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU56">
-        <f>(AS56&lt;$AT$1)*1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9782,7 +9782,7 @@
         <v>8.3994925166261794E-2</v>
       </c>
       <c r="AQ2">
-        <f>(AP2&lt;$AQ$1)*1</f>
+        <f t="shared" ref="AQ2:AQ33" si="0">(AP2&lt;$AQ$1)*1</f>
         <v>0</v>
       </c>
       <c r="AR2">
@@ -9917,7 +9917,7 @@
         <v>5.6641846335429701E-2</v>
       </c>
       <c r="AQ3">
-        <f>(AP3&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR3">
@@ -10052,7 +10052,7 @@
         <v>8.8119042975293105E-2</v>
       </c>
       <c r="AQ4">
-        <f>(AP4&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR4">
@@ -10187,7 +10187,7 @@
         <v>5.1630822461713098E-2</v>
       </c>
       <c r="AQ5">
-        <f>(AP5&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR5">
@@ -10322,7 +10322,7 @@
         <v>5.3359843103998203E-2</v>
       </c>
       <c r="AQ6">
-        <f>(AP6&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR6">
@@ -10457,7 +10457,7 @@
         <v>6.3965230661637701E-2</v>
       </c>
       <c r="AQ7">
-        <f>(AP7&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR7">
@@ -10592,7 +10592,7 @@
         <v>6.3294364174957096E-2</v>
       </c>
       <c r="AQ8">
-        <f>(AP8&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR8">
@@ -10727,7 +10727,7 @@
         <v>0.28743125122082702</v>
       </c>
       <c r="AQ9">
-        <f>(AP9&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR9">
@@ -10862,7 +10862,7 @@
         <v>8.8061347506270302E-2</v>
       </c>
       <c r="AQ10">
-        <f>(AP10&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR10">
@@ -10997,7 +10997,7 @@
         <v>8.5568368040426904E-2</v>
       </c>
       <c r="AQ11">
-        <f>(AP11&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR11">
@@ -11132,7 +11132,7 @@
         <v>5.2185812283075499E-2</v>
       </c>
       <c r="AQ12">
-        <f>(AP12&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR12">
@@ -11267,7 +11267,7 @@
         <v>4.07930099501344E-2</v>
       </c>
       <c r="AQ13">
-        <f>(AP13&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR13">
@@ -11402,7 +11402,7 @@
         <v>6.2676721024479007E-2</v>
       </c>
       <c r="AQ14">
-        <f>(AP14&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR14">
@@ -11537,7 +11537,7 @@
         <v>3.65379543615632E-2</v>
       </c>
       <c r="AQ15">
-        <f>(AP15&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR15">
@@ -11672,7 +11672,7 @@
         <v>7.3549860842136203E-2</v>
       </c>
       <c r="AQ16">
-        <f>(AP16&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR16">
@@ -11807,7 +11807,7 @@
         <v>5.5822524721224502E-2</v>
       </c>
       <c r="AQ17">
-        <f>(AP17&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR17">
@@ -11942,7 +11942,7 @@
         <v>5.5822524721224502E-2</v>
       </c>
       <c r="AQ18">
-        <f>(AP18&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR18">
@@ -12077,7 +12077,7 @@
         <v>5.5822524721224502E-2</v>
       </c>
       <c r="AQ19">
-        <f>(AP19&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR19">
@@ -12212,7 +12212,7 @@
         <v>4.3686306834502198E-2</v>
       </c>
       <c r="AQ20">
-        <f>(AP20&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR20">
@@ -12347,7 +12347,7 @@
         <v>7.7222342718796799E-2</v>
       </c>
       <c r="AQ21">
-        <f>(AP21&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR21">
@@ -12482,7 +12482,7 @@
         <v>4.3368801995537103E-2</v>
       </c>
       <c r="AQ22">
-        <f>(AP22&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR22">
@@ -12617,7 +12617,7 @@
         <v>7.9830994136638106E-2</v>
       </c>
       <c r="AQ23">
-        <f>(AP23&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR23">
@@ -12752,7 +12752,7 @@
         <v>5.6462882675500599E-2</v>
       </c>
       <c r="AQ24">
-        <f>(AP24&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR24">
@@ -12887,7 +12887,7 @@
         <v>3.84645236094995E-2</v>
       </c>
       <c r="AQ25">
-        <f>(AP25&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR25">
@@ -13022,7 +13022,7 @@
         <v>3.6157013157707203E-2</v>
       </c>
       <c r="AQ26">
-        <f>(AP26&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR26">
@@ -13157,7 +13157,7 @@
         <v>3.8274624403938098E-2</v>
       </c>
       <c r="AQ27">
-        <f>(AP27&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR27">
@@ -13292,7 +13292,7 @@
         <v>4.66987359960645E-2</v>
       </c>
       <c r="AQ28">
-        <f>(AP28&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR28">
@@ -13427,7 +13427,7 @@
         <v>5.6914205729780898E-2</v>
       </c>
       <c r="AQ29">
-        <f>(AP29&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AR29">
@@ -13562,7 +13562,7 @@
         <v>6.3470573245739598E-2</v>
       </c>
       <c r="AQ30">
-        <f>(AP30&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR30">
@@ -13697,7 +13697,7 @@
         <v>6.6678298859613197E-2</v>
       </c>
       <c r="AQ31">
-        <f>(AP31&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR31">
@@ -13832,7 +13832,7 @@
         <v>9.6720304183382205E-2</v>
       </c>
       <c r="AQ32">
-        <f>(AP32&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR32">
@@ -13967,7 +13967,7 @@
         <v>0.11114473526660899</v>
       </c>
       <c r="AQ33">
-        <f>(AP33&lt;$AQ$1)*1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR33">
@@ -14102,7 +14102,7 @@
         <v>0.147995323025013</v>
       </c>
       <c r="AQ34">
-        <f>(AP34&lt;$AQ$1)*1</f>
+        <f t="shared" ref="AQ34:AQ65" si="1">(AP34&lt;$AQ$1)*1</f>
         <v>0</v>
       </c>
       <c r="AR34">
@@ -14237,7 +14237,7 @@
         <v>0.19180444322124701</v>
       </c>
       <c r="AQ35">
-        <f>(AP35&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR35">
@@ -14372,7 +14372,7 @@
         <v>0.20198811808518799</v>
       </c>
       <c r="AQ36">
-        <f>(AP36&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR36">
@@ -14507,7 +14507,7 @@
         <v>6.3437593315102597E-2</v>
       </c>
       <c r="AQ37">
-        <f>(AP37&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR37">
@@ -14642,7 +14642,7 @@
         <v>0.12749842591633101</v>
       </c>
       <c r="AQ38">
-        <f>(AP38&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR38">
@@ -14777,7 +14777,7 @@
         <v>6.5636604147959507E-2</v>
       </c>
       <c r="AQ39">
-        <f>(AP39&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR39">
@@ -14912,7 +14912,7 @@
         <v>6.2307473545972297E-2</v>
       </c>
       <c r="AQ40">
-        <f>(AP40&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR40">
@@ -15047,7 +15047,7 @@
         <v>0.13741258492119701</v>
       </c>
       <c r="AQ41">
-        <f>(AP41&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR41">
@@ -15182,7 +15182,7 @@
         <v>6.2926704071356296E-2</v>
       </c>
       <c r="AQ42">
-        <f>(AP42&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR42">
@@ -15317,7 +15317,7 @@
         <v>0.132552474521974</v>
       </c>
       <c r="AQ43">
-        <f>(AP43&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR43">
@@ -15452,7 +15452,7 @@
         <v>0.162012510009993</v>
       </c>
       <c r="AQ44">
-        <f>(AP44&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR44">
@@ -15587,7 +15587,7 @@
         <v>5.0831197423612202E-2</v>
       </c>
       <c r="AQ45">
-        <f>(AP45&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AR45">
@@ -15722,7 +15722,7 @@
         <v>0.25372521030381101</v>
       </c>
       <c r="AQ46">
-        <f>(AP46&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR46">
@@ -15857,7 +15857,7 @@
         <v>0.31739119769346802</v>
       </c>
       <c r="AQ47">
-        <f>(AP47&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR47">
@@ -15992,7 +15992,7 @@
         <v>0.24892913365002001</v>
       </c>
       <c r="AQ48">
-        <f>(AP48&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR48">
@@ -16127,7 +16127,7 @@
         <v>4.2154989507924297E-2</v>
       </c>
       <c r="AQ49">
-        <f>(AP49&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AR49">
@@ -16262,7 +16262,7 @@
         <v>0.26140907316474299</v>
       </c>
       <c r="AQ50">
-        <f>(AP50&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR50">
@@ -16397,7 +16397,7 @@
         <v>0.32387986186974899</v>
       </c>
       <c r="AQ51">
-        <f>(AP51&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR51">
@@ -16532,7 +16532,7 @@
         <v>0.25644981079659401</v>
       </c>
       <c r="AQ52">
-        <f>(AP52&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR52">
@@ -16667,7 +16667,7 @@
         <v>0.25863238203201699</v>
       </c>
       <c r="AQ53">
-        <f>(AP53&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR53">
@@ -16802,7 +16802,7 @@
         <v>0.13291386810445099</v>
       </c>
       <c r="AQ54">
-        <f>(AP54&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR54">
@@ -16937,7 +16937,7 @@
         <v>5.3706315369040698E-2</v>
       </c>
       <c r="AQ55">
-        <f>(AP55&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AR55">
@@ -17072,7 +17072,7 @@
         <v>5.75586775269906E-2</v>
       </c>
       <c r="AQ56">
-        <f>(AP56&lt;$AQ$1)*1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AR56">

</xml_diff>